<commit_message>
TP#15399 Update ShipWorks to support FedEx Us Grn Alcohol
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/Grn Alcohol.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/Grn Alcohol.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Grn Alcohol" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_lu1">#REF!</definedName>
     <definedName name="_lu2">#REF!</definedName>
@@ -65,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="152">
   <si>
     <t>SaveLabel</t>
   </si>
@@ -511,6 +508,18 @@
   </si>
   <si>
     <t>HOME_DELIVERY_PREMIUM Each Package</t>
+  </si>
+  <si>
+    <t>20 Each Package</t>
+  </si>
+  <si>
+    <t>15 Each Package</t>
+  </si>
+  <si>
+    <t>100 Each Package</t>
+  </si>
+  <si>
+    <t>800</t>
   </si>
 </sst>
 </file>
@@ -902,116 +911,116 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1033,45 +1042,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover Page"/>
-      <sheetName val="Total Test Cases Count"/>
-      <sheetName val="US Exp Dom"/>
-      <sheetName val="US Exp Dom-Alcohol"/>
-      <sheetName val="US Exp Intl"/>
-      <sheetName val="US Exp Intl-Alcohol"/>
-      <sheetName val="US Grn Dom Intl And Home Del"/>
-      <sheetName val="Grn Alcohol"/>
-      <sheetName val="CA Exp Dom"/>
-      <sheetName val="CA Exp Intl"/>
-      <sheetName val="CA Grn Dom Intl"/>
-      <sheetName val="IMpB Smartpost test cases"/>
-      <sheetName val="ETD"/>
-      <sheetName val="OneRate"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1374,56 +1344,56 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:BQ10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BL1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D3" sqref="D3:D75"/>
-      <selection pane="bottomLeft" activeCell="AE4" sqref="AE4"/>
+      <selection pane="bottomLeft" activeCell="BO6" sqref="BO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="18" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="54" customWidth="1"/>
-    <col min="6" max="6" width="29" style="54" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="54" customWidth="1"/>
-    <col min="8" max="8" width="19" style="54" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="54" customWidth="1"/>
-    <col min="10" max="11" width="18.5703125" style="54" customWidth="1"/>
-    <col min="12" max="12" width="24" style="54" customWidth="1"/>
-    <col min="13" max="15" width="18.5703125" style="54" customWidth="1"/>
-    <col min="16" max="16" width="33.5703125" style="54" customWidth="1"/>
-    <col min="17" max="17" width="20" style="54" customWidth="1"/>
-    <col min="18" max="19" width="20.28515625" style="54" customWidth="1"/>
-    <col min="20" max="20" width="24" style="54" customWidth="1"/>
-    <col min="21" max="21" width="33.140625" style="54" customWidth="1"/>
-    <col min="22" max="22" width="20" style="54" customWidth="1"/>
-    <col min="23" max="24" width="20.28515625" style="54" customWidth="1"/>
-    <col min="25" max="27" width="57.85546875" style="54" customWidth="1"/>
-    <col min="28" max="28" width="51" style="54" customWidth="1"/>
-    <col min="29" max="29" width="50.7109375" style="54" customWidth="1"/>
-    <col min="30" max="31" width="51.5703125" style="54" customWidth="1"/>
-    <col min="32" max="33" width="40.42578125" style="54" customWidth="1"/>
-    <col min="34" max="34" width="49.140625" style="54" customWidth="1"/>
-    <col min="35" max="35" width="39.85546875" style="54" customWidth="1"/>
-    <col min="36" max="36" width="40.28515625" style="54" customWidth="1"/>
-    <col min="37" max="37" width="26.140625" style="54" customWidth="1"/>
-    <col min="38" max="38" width="19.7109375" style="54" customWidth="1"/>
-    <col min="39" max="39" width="19.5703125" style="54" customWidth="1"/>
-    <col min="40" max="42" width="24.140625" style="54" customWidth="1"/>
-    <col min="43" max="48" width="24.42578125" style="54" customWidth="1"/>
-    <col min="49" max="50" width="21.42578125" style="54" customWidth="1"/>
-    <col min="51" max="56" width="45.28515625" style="54" customWidth="1"/>
-    <col min="57" max="58" width="47.28515625" style="54" customWidth="1"/>
-    <col min="59" max="59" width="28.28515625" style="54" customWidth="1"/>
-    <col min="60" max="61" width="22.5703125" style="54" customWidth="1"/>
-    <col min="62" max="62" width="23.5703125" style="54" customWidth="1"/>
-    <col min="63" max="64" width="36.140625" style="54" customWidth="1"/>
-    <col min="65" max="65" width="51.28515625" style="54" customWidth="1"/>
-    <col min="66" max="67" width="61" style="54" customWidth="1"/>
-    <col min="68" max="68" width="50.7109375" style="54" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="51" customWidth="1"/>
+    <col min="6" max="6" width="29" style="51" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="19" style="51" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="51" customWidth="1"/>
+    <col min="10" max="11" width="18.5703125" style="51" customWidth="1"/>
+    <col min="12" max="12" width="24" style="51" customWidth="1"/>
+    <col min="13" max="15" width="18.5703125" style="51" customWidth="1"/>
+    <col min="16" max="16" width="33.5703125" style="51" customWidth="1"/>
+    <col min="17" max="17" width="20" style="51" customWidth="1"/>
+    <col min="18" max="19" width="20.28515625" style="51" customWidth="1"/>
+    <col min="20" max="20" width="24" style="51" customWidth="1"/>
+    <col min="21" max="21" width="33.140625" style="51" customWidth="1"/>
+    <col min="22" max="22" width="20" style="51" customWidth="1"/>
+    <col min="23" max="24" width="20.28515625" style="51" customWidth="1"/>
+    <col min="25" max="27" width="57.85546875" style="51" customWidth="1"/>
+    <col min="28" max="28" width="51" style="51" customWidth="1"/>
+    <col min="29" max="29" width="50.7109375" style="51" customWidth="1"/>
+    <col min="30" max="31" width="51.5703125" style="51" customWidth="1"/>
+    <col min="32" max="33" width="40.42578125" style="51" customWidth="1"/>
+    <col min="34" max="34" width="49.140625" style="51" customWidth="1"/>
+    <col min="35" max="35" width="39.85546875" style="51" customWidth="1"/>
+    <col min="36" max="36" width="40.28515625" style="51" customWidth="1"/>
+    <col min="37" max="37" width="26.140625" style="51" customWidth="1"/>
+    <col min="38" max="38" width="19.7109375" style="51" customWidth="1"/>
+    <col min="39" max="39" width="19.5703125" style="51" customWidth="1"/>
+    <col min="40" max="42" width="24.140625" style="51" customWidth="1"/>
+    <col min="43" max="48" width="24.42578125" style="51" customWidth="1"/>
+    <col min="49" max="50" width="21.42578125" style="51" customWidth="1"/>
+    <col min="51" max="56" width="45.28515625" style="51" customWidth="1"/>
+    <col min="57" max="58" width="47.28515625" style="51" customWidth="1"/>
+    <col min="59" max="59" width="28.28515625" style="51" customWidth="1"/>
+    <col min="60" max="61" width="22.5703125" style="51" customWidth="1"/>
+    <col min="62" max="62" width="23.5703125" style="51" customWidth="1"/>
+    <col min="63" max="64" width="36.140625" style="51" customWidth="1"/>
+    <col min="65" max="65" width="51.28515625" style="51" customWidth="1"/>
+    <col min="66" max="67" width="61" style="51" customWidth="1"/>
+    <col min="68" max="68" width="50.7109375" style="51" customWidth="1"/>
     <col min="69" max="69" width="18" style="18" bestFit="1" customWidth="1"/>
     <col min="70" max="16384" width="9.140625" style="18"/>
   </cols>
@@ -1835,1435 +1805,1435 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>270</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>605737</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24" t="s">
+      <c r="N3" s="23"/>
+      <c r="O3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="Q3" s="21">
         <v>151</v>
       </c>
-      <c r="R3" s="24" t="s">
+      <c r="R3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="S3" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="T3" s="24" t="s">
+      <c r="T3" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="U3" s="24">
+      <c r="U3" s="23">
         <v>38123</v>
       </c>
-      <c r="V3" s="24" t="s">
+      <c r="V3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="W3" s="24" t="s">
+      <c r="W3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="X3" s="25" t="s">
+      <c r="X3" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="Y3" s="26" t="s">
+      <c r="Y3" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="Z3" s="26" t="s">
+      <c r="Z3" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AA3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="AB3" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24" t="s">
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="AF3" s="24">
+      <c r="AF3" s="23">
         <v>71</v>
       </c>
-      <c r="AG3" s="27" t="s">
+      <c r="AG3" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="AH3" s="24" t="s">
+      <c r="AH3" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="28"/>
-      <c r="AP3" s="28"/>
-      <c r="AQ3" s="28"/>
-      <c r="AR3" s="28"/>
-      <c r="AS3" s="28"/>
-      <c r="AT3" s="28"/>
-      <c r="AU3" s="28"/>
-      <c r="AV3" s="28"/>
-      <c r="AW3" s="28"/>
-      <c r="AX3" s="28"/>
-      <c r="AY3" s="24">
-        <v>20</v>
-      </c>
-      <c r="AZ3" s="24">
-        <v>15</v>
-      </c>
-      <c r="BA3" s="24">
-        <v>20</v>
-      </c>
-      <c r="BB3" s="24" t="s">
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+      <c r="AQ3" s="27"/>
+      <c r="AR3" s="27"/>
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="27"/>
+      <c r="AU3" s="27"/>
+      <c r="AV3" s="27"/>
+      <c r="AW3" s="27"/>
+      <c r="AX3" s="27"/>
+      <c r="AY3" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ3" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA3" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="BB3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="BC3" s="24" t="s">
+      <c r="BC3" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="BD3" s="24" t="s">
+      <c r="BD3" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="BE3" s="24" t="s">
+      <c r="BE3" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="BF3" s="23">
-        <v>100</v>
-      </c>
-      <c r="BG3" s="24">
+      <c r="BF3" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG3" s="23">
         <v>2</v>
       </c>
-      <c r="BH3" s="24" t="s">
+      <c r="BH3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="BI3" s="24" t="s">
+      <c r="BI3" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="BJ3" s="24" t="s">
+      <c r="BJ3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="BK3" s="24">
+      <c r="BK3" s="23">
         <v>142</v>
       </c>
-      <c r="BL3" s="24" t="s">
+      <c r="BL3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="BM3" s="24"/>
-      <c r="BN3" s="24" t="s">
+      <c r="BM3" s="23"/>
+      <c r="BN3" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="BO3" s="28"/>
-      <c r="BP3" s="24" t="s">
+      <c r="BO3" s="27"/>
+      <c r="BP3" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="BQ3" s="29" t="s">
+      <c r="BQ3" s="28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32">
+      <c r="B4" s="54"/>
+      <c r="C4" s="30">
         <v>280</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="33">
         <v>605746</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="36" t="s">
+      <c r="L4" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="M4" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36" t="s">
+      <c r="N4" s="34"/>
+      <c r="O4" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P4" s="36" t="s">
+      <c r="P4" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="Q4" s="34">
+      <c r="Q4" s="32">
         <v>162</v>
       </c>
-      <c r="R4" s="36" t="s">
+      <c r="R4" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="S4" s="36" t="s">
+      <c r="S4" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="T4" s="36" t="s">
+      <c r="T4" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="U4" s="36" t="s">
+      <c r="U4" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="V4" s="36" t="s">
+      <c r="V4" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="W4" s="36" t="s">
+      <c r="W4" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="37">
-        <v>222327008</v>
-      </c>
-      <c r="Z4" s="37" t="s">
+      <c r="X4" s="34"/>
+      <c r="Y4" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z4" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AA4" s="37" t="s">
+      <c r="AA4" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AB4" s="36" t="s">
+      <c r="AB4" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36" t="s">
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="AE4" s="36" t="s">
+      <c r="AE4" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="AF4" s="36">
+      <c r="AF4" s="34">
         <v>69</v>
       </c>
-      <c r="AG4" s="38" t="s">
+      <c r="AG4" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH4" s="36">
+      <c r="AH4" s="34">
         <v>25</v>
       </c>
-      <c r="AI4" s="36" t="s">
+      <c r="AI4" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="AJ4" s="36" t="s">
+      <c r="AJ4" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="AK4" s="39">
+      <c r="AK4" s="37">
         <v>214877600</v>
       </c>
-      <c r="AL4" s="39" t="s">
+      <c r="AL4" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="AM4" s="39">
+      <c r="AM4" s="37">
         <v>123456789</v>
       </c>
-      <c r="AN4" s="39" t="s">
+      <c r="AN4" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AO4" s="39" t="s">
+      <c r="AO4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="AP4" s="39">
+      <c r="AP4" s="37">
         <v>9012633035</v>
       </c>
-      <c r="AQ4" s="36" t="s">
+      <c r="AQ4" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="AR4" s="36" t="s">
+      <c r="AR4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="AS4" s="36" t="s">
+      <c r="AS4" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="AT4" s="36" t="s">
+      <c r="AT4" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="AU4" s="39" t="s">
+      <c r="AU4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AV4" s="40" t="s">
+      <c r="AV4" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="AW4" s="39" t="s">
+      <c r="AW4" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="AX4" s="39"/>
-      <c r="AY4" s="36">
+      <c r="AX4" s="37"/>
+      <c r="AY4" s="34">
         <v>20</v>
       </c>
-      <c r="AZ4" s="36">
+      <c r="AZ4" s="34">
         <v>15</v>
       </c>
-      <c r="BA4" s="36">
+      <c r="BA4" s="34">
         <v>20</v>
       </c>
-      <c r="BB4" s="36" t="s">
+      <c r="BB4" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="BC4" s="36" t="s">
+      <c r="BC4" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="BD4" s="36" t="s">
+      <c r="BD4" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="BE4" s="36" t="s">
+      <c r="BE4" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="BF4" s="35">
-        <v>800</v>
-      </c>
-      <c r="BG4" s="36">
+      <c r="BF4" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="BG4" s="34">
         <v>1</v>
       </c>
-      <c r="BH4" s="36" t="s">
+      <c r="BH4" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="BI4" s="36" t="s">
+      <c r="BI4" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="BJ4" s="36" t="s">
+      <c r="BJ4" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="BK4" s="36">
+      <c r="BK4" s="34">
         <v>69</v>
       </c>
-      <c r="BL4" s="36" t="s">
+      <c r="BL4" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="BM4" s="36"/>
-      <c r="BN4" s="36" t="s">
+      <c r="BM4" s="34"/>
+      <c r="BN4" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="BO4" s="39"/>
-      <c r="BP4" s="36" t="s">
+      <c r="BO4" s="37"/>
+      <c r="BP4" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="BQ4" s="41" t="s">
+      <c r="BQ4" s="39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32">
+      <c r="B5" s="54"/>
+      <c r="C5" s="30">
         <v>281</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="33">
         <v>605749</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36" t="s">
+      <c r="N5" s="34"/>
+      <c r="O5" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="32">
         <v>165</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="T5" s="36" t="s">
+      <c r="T5" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="U5" s="36" t="s">
+      <c r="U5" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="V5" s="36" t="s">
+      <c r="V5" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="W5" s="36" t="s">
+      <c r="W5" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="37" t="s">
+      <c r="X5" s="40"/>
+      <c r="Y5" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="Z5" s="37" t="s">
+      <c r="Z5" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AA5" s="37" t="s">
+      <c r="AA5" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AB5" s="36" t="s">
+      <c r="AB5" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="36" t="s">
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="AE5" s="36" t="s">
+      <c r="AE5" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="AF5" s="36">
+      <c r="AF5" s="34">
         <v>50</v>
       </c>
-      <c r="AG5" s="38" t="s">
+      <c r="AG5" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH5" s="36">
+      <c r="AH5" s="34">
         <v>100</v>
       </c>
-      <c r="AI5" s="36" t="s">
+      <c r="AI5" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="AJ5" s="36" t="s">
+      <c r="AJ5" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="AK5" s="39">
+      <c r="AK5" s="37">
         <v>214877600</v>
       </c>
-      <c r="AL5" s="39" t="s">
+      <c r="AL5" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="AM5" s="39">
+      <c r="AM5" s="37">
         <v>123456789</v>
       </c>
-      <c r="AN5" s="39" t="s">
+      <c r="AN5" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AO5" s="39" t="s">
+      <c r="AO5" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="AP5" s="39">
+      <c r="AP5" s="37">
         <v>9012633035</v>
       </c>
-      <c r="AQ5" s="39" t="s">
+      <c r="AQ5" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="AR5" s="39" t="s">
+      <c r="AR5" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="AS5" s="39" t="s">
+      <c r="AS5" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="AT5" s="39" t="s">
+      <c r="AT5" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AU5" s="39" t="s">
+      <c r="AU5" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AV5" s="39" t="s">
+      <c r="AV5" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="AW5" s="39" t="s">
+      <c r="AW5" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="AX5" s="39" t="s">
+      <c r="AX5" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="AY5" s="36">
+      <c r="AY5" s="34">
         <v>20</v>
       </c>
-      <c r="AZ5" s="36">
+      <c r="AZ5" s="34">
         <v>15</v>
       </c>
-      <c r="BA5" s="36">
+      <c r="BA5" s="34">
         <v>20</v>
       </c>
-      <c r="BB5" s="36" t="s">
+      <c r="BB5" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="BC5" s="36" t="s">
+      <c r="BC5" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="BD5" s="36" t="s">
+      <c r="BD5" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="BE5" s="36" t="s">
+      <c r="BE5" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="BF5" s="35" t="s">
+      <c r="BF5" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="BG5" s="36">
+      <c r="BG5" s="34">
         <v>1</v>
       </c>
-      <c r="BH5" s="36" t="s">
+      <c r="BH5" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="BI5" s="36" t="s">
+      <c r="BI5" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="BJ5" s="36" t="s">
+      <c r="BJ5" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="BK5" s="36">
+      <c r="BK5" s="34">
         <v>50</v>
       </c>
-      <c r="BL5" s="36" t="s">
+      <c r="BL5" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="BM5" s="36"/>
-      <c r="BN5" s="36" t="s">
+      <c r="BM5" s="34"/>
+      <c r="BN5" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="BO5" s="39"/>
-      <c r="BP5" s="36" t="s">
+      <c r="BO5" s="37"/>
+      <c r="BP5" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="BQ5" s="41" t="s">
+      <c r="BQ5" s="39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32">
+      <c r="B6" s="54"/>
+      <c r="C6" s="30">
         <v>277</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="33">
         <v>605752</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="L6" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36" t="s">
+      <c r="N6" s="34"/>
+      <c r="O6" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P6" s="36" t="s">
+      <c r="P6" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="Q6" s="34">
+      <c r="Q6" s="32">
         <v>168</v>
       </c>
-      <c r="R6" s="36" t="s">
+      <c r="R6" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="S6" s="36" t="s">
+      <c r="S6" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="T6" s="36" t="s">
+      <c r="T6" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="U6" s="36" t="s">
+      <c r="U6" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="V6" s="36" t="s">
+      <c r="V6" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="W6" s="36" t="s">
+      <c r="W6" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="37">
+      <c r="X6" s="34"/>
+      <c r="Y6" s="35">
         <v>222326680</v>
       </c>
-      <c r="Z6" s="37" t="s">
+      <c r="Z6" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AA6" s="37" t="s">
+      <c r="AA6" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AB6" s="36" t="s">
+      <c r="AB6" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="AC6" s="36"/>
-      <c r="AD6" s="36" t="s">
+      <c r="AC6" s="34"/>
+      <c r="AD6" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="AE6" s="36" t="s">
+      <c r="AE6" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="AF6" s="36">
+      <c r="AF6" s="34">
         <v>50</v>
       </c>
-      <c r="AG6" s="38" t="s">
+      <c r="AG6" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH6" s="36">
+      <c r="AH6" s="34">
         <v>25</v>
       </c>
-      <c r="AI6" s="36" t="s">
+      <c r="AI6" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="AJ6" s="36" t="s">
+      <c r="AJ6" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="AK6" s="39">
+      <c r="AK6" s="37">
         <v>214877600</v>
       </c>
-      <c r="AL6" s="39" t="s">
+      <c r="AL6" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="AM6" s="39">
+      <c r="AM6" s="37">
         <v>123456789</v>
       </c>
-      <c r="AN6" s="39" t="s">
+      <c r="AN6" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="39" t="s">
+      <c r="AO6" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="AP6" s="39">
+      <c r="AP6" s="37">
         <v>9012633035</v>
       </c>
-      <c r="AQ6" s="34" t="s">
+      <c r="AQ6" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="AR6" s="34" t="s">
+      <c r="AR6" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="AS6" s="34" t="s">
+      <c r="AS6" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" s="34" t="s">
+      <c r="AT6" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="AU6" s="39" t="s">
+      <c r="AU6" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AV6" s="39"/>
-      <c r="AW6" s="39" t="s">
+      <c r="AV6" s="37"/>
+      <c r="AW6" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="AX6" s="39"/>
-      <c r="AY6" s="36">
+      <c r="AX6" s="37"/>
+      <c r="AY6" s="34">
         <v>20</v>
       </c>
-      <c r="AZ6" s="36">
+      <c r="AZ6" s="34">
         <v>15</v>
       </c>
-      <c r="BA6" s="36">
+      <c r="BA6" s="34">
         <v>20</v>
       </c>
-      <c r="BB6" s="36" t="s">
+      <c r="BB6" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="BC6" s="36" t="s">
+      <c r="BC6" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="BD6" s="36" t="s">
+      <c r="BD6" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="BE6" s="36" t="s">
+      <c r="BE6" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="BF6" s="35" t="s">
+      <c r="BF6" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="BG6" s="36">
+      <c r="BG6" s="34">
         <v>1</v>
       </c>
-      <c r="BH6" s="36" t="s">
+      <c r="BH6" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="BI6" s="36" t="s">
+      <c r="BI6" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="BJ6" s="36" t="s">
+      <c r="BJ6" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="BK6" s="36">
+      <c r="BK6" s="34">
         <v>50</v>
       </c>
-      <c r="BL6" s="36" t="s">
+      <c r="BL6" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="BM6" s="36"/>
-      <c r="BN6" s="36" t="s">
+      <c r="BM6" s="34"/>
+      <c r="BN6" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="BO6" s="39"/>
-      <c r="BP6" s="36" t="s">
+      <c r="BO6" s="37"/>
+      <c r="BP6" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="BQ6" s="41" t="s">
+      <c r="BQ6" s="39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32">
+      <c r="B7" s="54"/>
+      <c r="C7" s="30">
         <v>770</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="33">
         <v>605766</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="J7" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="36" t="s">
+      <c r="K7" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="36" t="s">
+      <c r="L7" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="36" t="s">
+      <c r="M7" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36" t="s">
+      <c r="N7" s="34"/>
+      <c r="O7" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P7" s="36" t="s">
+      <c r="P7" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="Q7" s="34">
+      <c r="Q7" s="32">
         <v>883</v>
       </c>
-      <c r="R7" s="36" t="s">
+      <c r="R7" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="S7" s="36" t="s">
+      <c r="S7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="T7" s="36" t="s">
+      <c r="T7" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="U7" s="36" t="s">
+      <c r="U7" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="V7" s="36" t="s">
+      <c r="V7" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="W7" s="36" t="s">
+      <c r="W7" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="X7" s="42" t="s">
+      <c r="X7" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="Y7" s="37" t="s">
+      <c r="Y7" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="Z7" s="37" t="s">
+      <c r="Z7" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AA7" s="37" t="s">
+      <c r="AA7" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AB7" s="36" t="s">
+      <c r="AB7" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="AC7" s="36"/>
-      <c r="AD7" s="36" t="s">
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="AE7" s="36" t="s">
+      <c r="AE7" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="AF7" s="36">
+      <c r="AF7" s="34">
         <v>70</v>
       </c>
-      <c r="AG7" s="38" t="s">
+      <c r="AG7" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH7" s="36" t="s">
+      <c r="AH7" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AI7" s="36"/>
-      <c r="AJ7" s="36"/>
-      <c r="AK7" s="39"/>
-      <c r="AL7" s="39"/>
-      <c r="AM7" s="39"/>
-      <c r="AN7" s="39"/>
-      <c r="AO7" s="39"/>
-      <c r="AP7" s="39"/>
-      <c r="AQ7" s="39"/>
-      <c r="AR7" s="39"/>
-      <c r="AS7" s="39"/>
-      <c r="AT7" s="39"/>
-      <c r="AU7" s="39"/>
-      <c r="AV7" s="39"/>
-      <c r="AW7" s="39"/>
-      <c r="AX7" s="39"/>
-      <c r="AY7" s="36">
+      <c r="AI7" s="34"/>
+      <c r="AJ7" s="34"/>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37"/>
+      <c r="AM7" s="37"/>
+      <c r="AN7" s="37"/>
+      <c r="AO7" s="37"/>
+      <c r="AP7" s="37"/>
+      <c r="AQ7" s="37"/>
+      <c r="AR7" s="37"/>
+      <c r="AS7" s="37"/>
+      <c r="AT7" s="37"/>
+      <c r="AU7" s="37"/>
+      <c r="AV7" s="37"/>
+      <c r="AW7" s="37"/>
+      <c r="AX7" s="37"/>
+      <c r="AY7" s="34">
         <v>20</v>
       </c>
-      <c r="AZ7" s="36">
+      <c r="AZ7" s="34">
         <v>20</v>
       </c>
-      <c r="BA7" s="36" t="s">
+      <c r="BA7" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="BB7" s="36" t="s">
+      <c r="BB7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="BC7" s="36" t="s">
+      <c r="BC7" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="BD7" s="36" t="s">
+      <c r="BD7" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="BE7" s="36" t="s">
+      <c r="BE7" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="BF7" s="35" t="s">
+      <c r="BF7" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="BG7" s="36">
+      <c r="BG7" s="34">
         <v>1</v>
       </c>
-      <c r="BH7" s="36" t="s">
+      <c r="BH7" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="BI7" s="36" t="s">
+      <c r="BI7" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="BJ7" s="36" t="s">
+      <c r="BJ7" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="BK7" s="36">
+      <c r="BK7" s="34">
         <v>70</v>
       </c>
-      <c r="BL7" s="36" t="s">
+      <c r="BL7" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="BM7" s="36" t="s">
+      <c r="BM7" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="BN7" s="36"/>
-      <c r="BO7" s="36" t="s">
+      <c r="BN7" s="34"/>
+      <c r="BO7" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="BP7" s="36" t="s">
+      <c r="BP7" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="BQ7" s="41" t="s">
+      <c r="BQ7" s="39" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32">
+      <c r="B8" s="54"/>
+      <c r="C8" s="30">
         <v>780</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="33">
         <v>605772</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="L8" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="M8" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36" t="s">
+      <c r="N8" s="34"/>
+      <c r="O8" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="P8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="34">
+      <c r="Q8" s="32">
         <v>889</v>
       </c>
-      <c r="R8" s="36" t="s">
+      <c r="R8" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="36" t="s">
+      <c r="S8" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="T8" s="36" t="s">
+      <c r="T8" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="U8" s="36" t="s">
+      <c r="U8" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="V8" s="36" t="s">
+      <c r="V8" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="W8" s="36" t="s">
+      <c r="W8" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="X8" s="42" t="s">
+      <c r="X8" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="Y8" s="35" t="s">
+      <c r="Y8" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="Z8" s="37" t="s">
+      <c r="Z8" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AA8" s="37" t="s">
+      <c r="AA8" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AB8" s="36" t="s">
+      <c r="AB8" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="36" t="s">
+      <c r="AC8" s="34"/>
+      <c r="AD8" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="AE8" s="36" t="s">
+      <c r="AE8" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="AF8" s="36">
+      <c r="AF8" s="34">
         <v>60</v>
       </c>
-      <c r="AG8" s="38" t="s">
+      <c r="AG8" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH8" s="36" t="s">
+      <c r="AH8" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AI8" s="36"/>
-      <c r="AJ8" s="36"/>
-      <c r="AK8" s="39"/>
-      <c r="AL8" s="39"/>
-      <c r="AM8" s="39"/>
-      <c r="AN8" s="39"/>
-      <c r="AO8" s="39"/>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="39"/>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="39"/>
-      <c r="AT8" s="39"/>
-      <c r="AU8" s="39"/>
-      <c r="AV8" s="39"/>
-      <c r="AW8" s="39"/>
-      <c r="AX8" s="39"/>
-      <c r="AY8" s="36">
+      <c r="AI8" s="34"/>
+      <c r="AJ8" s="34"/>
+      <c r="AK8" s="37"/>
+      <c r="AL8" s="37"/>
+      <c r="AM8" s="37"/>
+      <c r="AN8" s="37"/>
+      <c r="AO8" s="37"/>
+      <c r="AP8" s="37"/>
+      <c r="AQ8" s="37"/>
+      <c r="AR8" s="37"/>
+      <c r="AS8" s="37"/>
+      <c r="AT8" s="37"/>
+      <c r="AU8" s="37"/>
+      <c r="AV8" s="37"/>
+      <c r="AW8" s="37"/>
+      <c r="AX8" s="37"/>
+      <c r="AY8" s="34">
         <v>20</v>
       </c>
-      <c r="AZ8" s="36">
+      <c r="AZ8" s="34">
         <v>15</v>
       </c>
-      <c r="BA8" s="36">
+      <c r="BA8" s="34">
         <v>20</v>
       </c>
-      <c r="BB8" s="36" t="s">
+      <c r="BB8" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="BC8" s="36" t="s">
+      <c r="BC8" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="BD8" s="36" t="s">
+      <c r="BD8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="BE8" s="36" t="s">
+      <c r="BE8" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="BF8" s="35" t="s">
+      <c r="BF8" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="BG8" s="36">
+      <c r="BG8" s="34">
         <v>1</v>
       </c>
-      <c r="BH8" s="36" t="s">
+      <c r="BH8" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="BI8" s="36" t="s">
+      <c r="BI8" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="BJ8" s="36" t="s">
+      <c r="BJ8" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="BK8" s="36">
+      <c r="BK8" s="34">
         <v>60</v>
       </c>
-      <c r="BL8" s="36" t="s">
+      <c r="BL8" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="BM8" s="36" t="s">
+      <c r="BM8" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="BN8" s="36" t="s">
+      <c r="BN8" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="BO8" s="36" t="s">
+      <c r="BO8" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="BP8" s="36" t="s">
+      <c r="BP8" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="BQ8" s="41" t="s">
+      <c r="BQ8" s="39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32">
+      <c r="B9" s="54"/>
+      <c r="C9" s="30">
         <v>777</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="33">
         <v>605776</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="M9" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36" t="s">
+      <c r="N9" s="34"/>
+      <c r="O9" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="Q9" s="34">
+      <c r="Q9" s="32">
         <v>893</v>
       </c>
-      <c r="R9" s="36" t="s">
+      <c r="R9" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="S9" s="36" t="s">
+      <c r="S9" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="T9" s="36" t="s">
+      <c r="T9" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="U9" s="36" t="s">
+      <c r="U9" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="V9" s="36" t="s">
+      <c r="V9" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="W9" s="36" t="s">
+      <c r="W9" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="X9" s="42" t="s">
+      <c r="X9" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="Y9" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z9" s="37" t="s">
+      <c r="Y9" s="33">
+        <v>222327008</v>
+      </c>
+      <c r="Z9" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="AA9" s="37" t="s">
+      <c r="AA9" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="AB9" s="35" t="s">
+      <c r="AB9" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36" t="s">
+      <c r="AC9" s="34"/>
+      <c r="AD9" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="AE9" s="36" t="s">
+      <c r="AE9" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="AF9" s="36">
+      <c r="AF9" s="34">
         <v>20</v>
       </c>
-      <c r="AG9" s="38" t="s">
+      <c r="AG9" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="AH9" s="36" t="s">
+      <c r="AH9" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AI9" s="36"/>
-      <c r="AJ9" s="36"/>
-      <c r="AK9" s="39"/>
-      <c r="AL9" s="39"/>
-      <c r="AM9" s="39"/>
-      <c r="AN9" s="39"/>
-      <c r="AO9" s="39"/>
-      <c r="AP9" s="39"/>
-      <c r="AQ9" s="39"/>
-      <c r="AR9" s="39"/>
-      <c r="AS9" s="39"/>
-      <c r="AT9" s="39"/>
-      <c r="AU9" s="39"/>
-      <c r="AV9" s="39"/>
-      <c r="AW9" s="39"/>
-      <c r="AX9" s="39"/>
-      <c r="AY9" s="36">
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
+      <c r="AK9" s="37"/>
+      <c r="AL9" s="37"/>
+      <c r="AM9" s="37"/>
+      <c r="AN9" s="37"/>
+      <c r="AO9" s="37"/>
+      <c r="AP9" s="37"/>
+      <c r="AQ9" s="37"/>
+      <c r="AR9" s="37"/>
+      <c r="AS9" s="37"/>
+      <c r="AT9" s="37"/>
+      <c r="AU9" s="37"/>
+      <c r="AV9" s="37"/>
+      <c r="AW9" s="37"/>
+      <c r="AX9" s="37"/>
+      <c r="AY9" s="34">
         <v>20</v>
       </c>
-      <c r="AZ9" s="36">
+      <c r="AZ9" s="34">
         <v>15</v>
       </c>
-      <c r="BA9" s="36">
+      <c r="BA9" s="34">
         <v>20</v>
       </c>
-      <c r="BB9" s="36" t="s">
+      <c r="BB9" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="BC9" s="36" t="s">
+      <c r="BC9" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="BD9" s="36" t="s">
+      <c r="BD9" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="BE9" s="36" t="s">
+      <c r="BE9" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="BF9" s="35" t="s">
+      <c r="BF9" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="BG9" s="36">
+      <c r="BG9" s="34">
         <v>1</v>
       </c>
-      <c r="BH9" s="36" t="s">
+      <c r="BH9" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="BI9" s="36" t="s">
+      <c r="BI9" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="BJ9" s="36" t="s">
+      <c r="BJ9" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="BK9" s="36">
+      <c r="BK9" s="34">
         <v>20</v>
       </c>
-      <c r="BL9" s="36" t="s">
+      <c r="BL9" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="BM9" s="36" t="s">
+      <c r="BM9" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="BN9" s="36" t="s">
+      <c r="BN9" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="BO9" s="36" t="s">
+      <c r="BO9" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="BP9" s="39" t="s">
+      <c r="BP9" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="BQ9" s="41" t="s">
+      <c r="BQ9" s="39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:69" s="30" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" s="29" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44">
+      <c r="B10" s="55"/>
+      <c r="C10" s="41">
         <v>776</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="44">
         <v>605777</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="48" t="s">
+      <c r="H10" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="J10" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="K10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="M10" s="48" t="s">
+      <c r="M10" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48" t="s">
+      <c r="N10" s="45"/>
+      <c r="O10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="P10" s="48" t="s">
+      <c r="P10" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" s="46">
+      <c r="Q10" s="43">
         <v>894</v>
       </c>
-      <c r="R10" s="48" t="s">
+      <c r="R10" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="S10" s="48" t="s">
+      <c r="S10" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="T10" s="48" t="s">
+      <c r="T10" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="U10" s="48" t="s">
+      <c r="U10" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="V10" s="48" t="s">
+      <c r="V10" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="W10" s="48" t="s">
+      <c r="W10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="X10" s="49" t="s">
+      <c r="X10" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="Y10" s="50">
+      <c r="Y10" s="47">
         <v>222327008</v>
       </c>
-      <c r="Z10" s="50" t="s">
+      <c r="Z10" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AA10" s="50" t="s">
+      <c r="AA10" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="AB10" s="47" t="s">
+      <c r="AB10" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="AC10" s="48"/>
-      <c r="AD10" s="48" t="s">
+      <c r="AC10" s="45"/>
+      <c r="AD10" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="AE10" s="48" t="s">
+      <c r="AE10" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="AF10" s="48">
+      <c r="AF10" s="45">
         <v>50</v>
       </c>
-      <c r="AG10" s="51" t="s">
+      <c r="AG10" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="AH10" s="48" t="s">
+      <c r="AH10" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="AI10" s="48"/>
-      <c r="AJ10" s="48"/>
-      <c r="AK10" s="52"/>
-      <c r="AL10" s="52"/>
-      <c r="AM10" s="52"/>
-      <c r="AN10" s="52"/>
-      <c r="AO10" s="52"/>
-      <c r="AP10" s="52"/>
-      <c r="AQ10" s="52"/>
-      <c r="AR10" s="52"/>
-      <c r="AS10" s="52"/>
-      <c r="AT10" s="52"/>
-      <c r="AU10" s="52"/>
-      <c r="AV10" s="52"/>
-      <c r="AW10" s="52"/>
-      <c r="AX10" s="52"/>
-      <c r="AY10" s="48">
-        <v>20</v>
-      </c>
-      <c r="AZ10" s="48">
-        <v>15</v>
-      </c>
-      <c r="BA10" s="48">
-        <v>20</v>
-      </c>
-      <c r="BB10" s="48" t="s">
+      <c r="AI10" s="45"/>
+      <c r="AJ10" s="45"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="49"/>
+      <c r="AM10" s="49"/>
+      <c r="AN10" s="49"/>
+      <c r="AO10" s="49"/>
+      <c r="AP10" s="49"/>
+      <c r="AQ10" s="49"/>
+      <c r="AR10" s="49"/>
+      <c r="AS10" s="49"/>
+      <c r="AT10" s="49"/>
+      <c r="AU10" s="49"/>
+      <c r="AV10" s="49"/>
+      <c r="AW10" s="49"/>
+      <c r="AX10" s="49"/>
+      <c r="AY10" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ10" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA10" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="BB10" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="BC10" s="48" t="s">
+      <c r="BC10" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="BD10" s="48" t="s">
+      <c r="BD10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="BE10" s="48" t="s">
+      <c r="BE10" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="BF10" s="47">
+      <c r="BF10" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG10" s="45">
+        <v>2</v>
+      </c>
+      <c r="BH10" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="BI10" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ10" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="BK10" s="45">
         <v>100</v>
       </c>
-      <c r="BG10" s="48">
-        <v>2</v>
-      </c>
-      <c r="BH10" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="BI10" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="BJ10" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="BK10" s="48">
-        <v>50</v>
-      </c>
-      <c r="BL10" s="48" t="s">
+      <c r="BL10" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="BM10" s="48" t="s">
+      <c r="BM10" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="BN10" s="48"/>
-      <c r="BO10" s="48" t="s">
+      <c r="BN10" s="45"/>
+      <c r="BO10" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="BP10" s="52" t="s">
+      <c r="BP10" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="BQ10" s="53" t="s">
+      <c r="BQ10" s="50" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TP#20088:  Updating FedEx cert tests for 2017
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/Grn Alcohol.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/Grn Alcohol.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="163">
   <si>
     <t>GUARANTEED_FUNDS</t>
   </si>
@@ -2303,10 +2303,10 @@
   </sheetPr>
   <dimension ref="A1:BT13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BL1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="BT11" sqref="BT11"/>
+      <selection pane="bottomLeft" activeCell="BQ2" sqref="BQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2906,7 +2906,9 @@
       <c r="AS3" s="25"/>
       <c r="AT3" s="25"/>
       <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
+      <c r="AV3" s="32">
+        <v>9012633035</v>
+      </c>
       <c r="AW3" s="25"/>
       <c r="AX3" s="25"/>
       <c r="AY3" s="25"/>
@@ -2949,7 +2951,9 @@
       <c r="BP3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="BQ3" s="25"/>
+      <c r="BQ3" s="29" t="s">
+        <v>16</v>
+      </c>
       <c r="BR3" s="22" t="s">
         <v>108</v>
       </c>
@@ -3153,7 +3157,9 @@
       <c r="BP4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="BQ4" s="32"/>
+      <c r="BQ4" s="29" t="s">
+        <v>16</v>
+      </c>
       <c r="BR4" s="29" t="s">
         <v>108</v>
       </c>
@@ -3353,7 +3359,9 @@
       <c r="BP5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="BQ5" s="32"/>
+      <c r="BQ5" s="29" t="s">
+        <v>16</v>
+      </c>
       <c r="BR5" s="29" t="s">
         <v>108</v>
       </c>
@@ -3484,7 +3492,9 @@
       <c r="AS6" s="32"/>
       <c r="AT6" s="32"/>
       <c r="AU6" s="32"/>
-      <c r="AV6" s="32"/>
+      <c r="AV6" s="32">
+        <v>9012633035</v>
+      </c>
       <c r="AW6" s="32"/>
       <c r="AX6" s="32"/>
       <c r="AY6" s="32"/>
@@ -3527,7 +3537,9 @@
         <v>53</v>
       </c>
       <c r="BP6" s="29"/>
-      <c r="BQ6" s="29"/>
+      <c r="BQ6" s="29" t="s">
+        <v>16</v>
+      </c>
       <c r="BR6" s="29" t="s">
         <v>108</v>
       </c>
@@ -3658,7 +3670,9 @@
       <c r="AS7" s="32"/>
       <c r="AT7" s="32"/>
       <c r="AU7" s="32"/>
-      <c r="AV7" s="32"/>
+      <c r="AV7" s="32">
+        <v>9012633035</v>
+      </c>
       <c r="AW7" s="32"/>
       <c r="AX7" s="32"/>
       <c r="AY7" s="32"/>
@@ -3836,7 +3850,9 @@
       <c r="AS8" s="32"/>
       <c r="AT8" s="32"/>
       <c r="AU8" s="32"/>
-      <c r="AV8" s="32"/>
+      <c r="AV8" s="32">
+        <v>9012633035</v>
+      </c>
       <c r="AW8" s="32"/>
       <c r="AX8" s="32"/>
       <c r="AY8" s="32"/>
@@ -4014,7 +4030,9 @@
       <c r="AS9" s="43"/>
       <c r="AT9" s="43"/>
       <c r="AU9" s="43"/>
-      <c r="AV9" s="43"/>
+      <c r="AV9" s="32">
+        <v>9012633035</v>
+      </c>
       <c r="AW9" s="43"/>
       <c r="AX9" s="43"/>
       <c r="AY9" s="43"/>

</xml_diff>